<commit_message>
einige Bauteile geändert, so dass sie Basic Parts bei JLC sind
</commit_message>
<xml_diff>
--- a/gsvesc-jlcbom.xlsx
+++ b/gsvesc-jlcbom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="135">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">C1794</t>
   </si>
   <si>
+    <t xml:space="preserve">13/7.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">10u0/25V</t>
   </si>
   <si>
@@ -115,6 +118,9 @@
     <t xml:space="preserve">C46653</t>
   </si>
   <si>
+    <t xml:space="preserve">R1</t>
+  </si>
+  <si>
     <t xml:space="preserve">BLUE</t>
   </si>
   <si>
@@ -124,6 +130,9 @@
     <t xml:space="preserve">C2293</t>
   </si>
   <si>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
     <t xml:space="preserve">RED</t>
   </si>
   <si>
@@ -139,6 +148,9 @@
     <t xml:space="preserve">C2297</t>
   </si>
   <si>
+    <t xml:space="preserve">Verhältnis</t>
+  </si>
+  <si>
     <t xml:space="preserve">SS210</t>
   </si>
   <si>
@@ -163,6 +175,18 @@
     <t xml:space="preserve">C8598</t>
   </si>
   <si>
+    <t xml:space="preserve">SMMBD914LT3G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D8, D9, D10,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT-23-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C233426</t>
+  </si>
+  <si>
     <t xml:space="preserve">470u</t>
   </si>
   <si>
@@ -238,7 +262,7 @@
     <t xml:space="preserve">10k0</t>
   </si>
   <si>
-    <t xml:space="preserve">R8, R16, R27, R36, R41</t>
+    <t xml:space="preserve">R8, R16,  R36, R41</t>
   </si>
   <si>
     <t xml:space="preserve">C17414</t>
@@ -253,6 +277,15 @@
     <t xml:space="preserve">C17513</t>
   </si>
   <si>
+    <t xml:space="preserve">13k0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17455</t>
+  </si>
+  <si>
     <t xml:space="preserve">221R</t>
   </si>
   <si>
@@ -301,13 +334,13 @@
     <t xml:space="preserve">C76233</t>
   </si>
   <si>
-    <t xml:space="preserve">5k90</t>
+    <t xml:space="preserve">7k50</t>
   </si>
   <si>
     <t xml:space="preserve">R34, </t>
   </si>
   <si>
-    <t xml:space="preserve">C17730</t>
+    <t xml:space="preserve">C17807</t>
   </si>
   <si>
     <t xml:space="preserve">STM32F405RGT6</t>
@@ -382,7 +415,7 @@
     <t xml:space="preserve">C9864</t>
   </si>
   <si>
-    <t xml:space="preserve">ABM3B 8MHz</t>
+    <t xml:space="preserve">X50328MSB2GI</t>
   </si>
   <si>
     <t xml:space="preserve">Y1, </t>
@@ -391,7 +424,7 @@
     <t xml:space="preserve">SMD-4</t>
   </si>
   <si>
-    <t xml:space="preserve">C83312</t>
+    <t xml:space="preserve">C115962</t>
   </si>
 </sst>
 </file>
@@ -402,11 +435,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -428,6 +462,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -441,21 +476,10 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -528,15 +552,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -557,16 +581,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ36"/>
+  <dimension ref="A1:AMJ38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.02"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
@@ -617,467 +641,528 @@
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="H3" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>7.5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <f aca="false">H10/H9</f>
+        <v>0.59</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <f aca="false">J10/J9</f>
+        <v>0.576923076923077</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <f aca="false">K12-H12</f>
+        <v>-0.0130769230769232</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>50</v>
+      <c r="A15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>57</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>64</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>64</v>
+      <c r="D19" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>67</v>
+      <c r="D20" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>70</v>
+      <c r="D21" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>73</v>
+      <c r="D22" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>85</v>
+      <c r="D26" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>88</v>
+      <c r="D27" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>92</v>
+        <v>6</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>95</v>
+      <c r="D29" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>121</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>125</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>123</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1095,28 +1180,30 @@
     <hyperlink ref="D12" r:id="rId11" display="C2297"/>
     <hyperlink ref="D13" r:id="rId12" display="C14996"/>
     <hyperlink ref="D14" r:id="rId13" display="C8598"/>
-    <hyperlink ref="D15" r:id="rId14" display="C169393"/>
-    <hyperlink ref="D16" r:id="rId15" display="C132136"/>
-    <hyperlink ref="D17" r:id="rId16" display="C146377"/>
-    <hyperlink ref="D18" r:id="rId17" display="C17477"/>
-    <hyperlink ref="D19" r:id="rId18" display="C17561"/>
-    <hyperlink ref="D20" r:id="rId19" display="C17408"/>
-    <hyperlink ref="D21" r:id="rId20" display="C17530"/>
-    <hyperlink ref="D22" r:id="rId21" display="C17414"/>
-    <hyperlink ref="D23" r:id="rId22" display="C17513"/>
-    <hyperlink ref="D24" r:id="rId23" display="C17557"/>
-    <hyperlink ref="D25" r:id="rId24" display="C17772"/>
-    <hyperlink ref="D26" r:id="rId25" display="C4382"/>
-    <hyperlink ref="D27" r:id="rId26" display="C17675"/>
-    <hyperlink ref="D28" r:id="rId27" display="C76233"/>
-    <hyperlink ref="D29" r:id="rId28" display="C17730"/>
-    <hyperlink ref="D30" r:id="rId29" display="C15742"/>
-    <hyperlink ref="D31" r:id="rId30" display="C129332"/>
-    <hyperlink ref="D32" r:id="rId31" display="C129949"/>
-    <hyperlink ref="D33" r:id="rId32" display="C9424"/>
-    <hyperlink ref="D34" r:id="rId33" display="C133643"/>
-    <hyperlink ref="D35" r:id="rId34" display="C9864"/>
-    <hyperlink ref="D36" r:id="rId35" display="C83312"/>
+    <hyperlink ref="D15" r:id="rId14" display="C233426"/>
+    <hyperlink ref="D16" r:id="rId15" display="C169393"/>
+    <hyperlink ref="D17" r:id="rId16" display="C132136"/>
+    <hyperlink ref="D18" r:id="rId17" display="C146377"/>
+    <hyperlink ref="D19" r:id="rId18" display="C17477"/>
+    <hyperlink ref="D20" r:id="rId19" display="C17561"/>
+    <hyperlink ref="D21" r:id="rId20" display="C17408"/>
+    <hyperlink ref="D22" r:id="rId21" display="C17530"/>
+    <hyperlink ref="D23" r:id="rId22" display="C17414"/>
+    <hyperlink ref="D24" r:id="rId23" display="C17513"/>
+    <hyperlink ref="D25" r:id="rId24" display="C17455"/>
+    <hyperlink ref="D26" r:id="rId25" display="C17557"/>
+    <hyperlink ref="D27" r:id="rId26" display="C17772"/>
+    <hyperlink ref="D28" r:id="rId27" display="C4382"/>
+    <hyperlink ref="D29" r:id="rId28" display="C17675"/>
+    <hyperlink ref="D30" r:id="rId29" display="C76233"/>
+    <hyperlink ref="D31" r:id="rId30" display="C17807"/>
+    <hyperlink ref="D32" r:id="rId31" display="C15742"/>
+    <hyperlink ref="D33" r:id="rId32" display="C129332"/>
+    <hyperlink ref="D34" r:id="rId33" display="C129949"/>
+    <hyperlink ref="D35" r:id="rId34" display="C9424"/>
+    <hyperlink ref="D36" r:id="rId35" display="C133643"/>
+    <hyperlink ref="D37" r:id="rId36" display="C9864"/>
+    <hyperlink ref="D38" r:id="rId37" display="C115962"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>